<commit_message>
New results xls and teleport keyword taken out.
</commit_message>
<xml_diff>
--- a/Stats_New.xlsx
+++ b/Stats_New.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
   <si>
     <t>Scenario</t>
   </si>
@@ -90,9 +90,6 @@
     <t>1 T / 6 C</t>
   </si>
   <si>
-    <t xml:space="preserve">This is about as far as we can go. After this, things just don't work well and programs lag and I think are just being overwhemed by the speed at which packets are coming in. </t>
-  </si>
-  <si>
     <t>Note: These numbers are gathered after 5 minutes.</t>
   </si>
   <si>
@@ -112,6 +109,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Note: 10 ms was too high here, so we backed it off to 100ms</t>
+  </si>
+  <si>
+    <t>C 7</t>
   </si>
 </sst>
 </file>
@@ -173,8 +176,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -201,7 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -211,6 +218,8 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -220,6 +229,8 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -549,11 +560,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M58"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -574,7 +585,7 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -607,13 +618,13 @@
         <v>8</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>5</v>
@@ -622,10 +633,10 @@
         <v>6</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1">
@@ -638,10 +649,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="2">
         <v>8.7800000000000003E-2</v>
@@ -762,15 +773,15 @@
         <v>11526</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" ref="J10:J39" si="0">F11/E11</f>
+        <f t="shared" ref="J11:J39" si="0">F11/E11</f>
         <v>0.26170744693164194</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" ref="K10:K39" si="1">G11/E11</f>
+        <f t="shared" ref="K11:K39" si="1">G11/E11</f>
         <v>0.73829255306835806</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" ref="L10:L39" si="2">H11/G11</f>
+        <f t="shared" ref="L11:L39" si="2">H11/G11</f>
         <v>0</v>
       </c>
       <c r="M11" s="2">
@@ -972,49 +983,98 @@
       <c r="A17" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="J17" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K17" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L17" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M17" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B17">
+        <v>1.14365E-3</v>
+      </c>
+      <c r="C17">
+        <v>1.5509E-3</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.2263</v>
+      </c>
+      <c r="E17">
+        <v>227921</v>
+      </c>
+      <c r="F17">
+        <v>34361</v>
+      </c>
+      <c r="G17">
+        <v>193560</v>
+      </c>
+      <c r="H17">
+        <v>3496</v>
+      </c>
+      <c r="I17">
+        <v>50813</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15075837680599857</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="1"/>
+        <v>0.84924162319400143</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="2"/>
+        <v>1.8061582971688365E-2</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="3"/>
+        <v>0.26251808224839845</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="J18" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K18" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L18" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M18" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B18">
+        <v>1.5419299999999999E-3</v>
+      </c>
+      <c r="C18">
+        <v>2.0166799999999999E-3</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.1111</v>
+      </c>
+      <c r="E18">
+        <v>248058</v>
+      </c>
+      <c r="F18">
+        <v>19955</v>
+      </c>
+      <c r="G18">
+        <v>228103</v>
+      </c>
+      <c r="H18">
+        <v>4577</v>
+      </c>
+      <c r="I18">
+        <v>61090</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="0"/>
+        <v>8.044489595175322E-2</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="1"/>
+        <v>0.91955510404824681</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="2"/>
+        <v>2.0065496727355626E-2</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="3"/>
+        <v>0.26781760871185384</v>
       </c>
     </row>
     <row r="19" spans="1:13" s="3" customFormat="1">
       <c r="A19" s="3" t="s">
         <v>15</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D19" s="4"/>
       <c r="J19" s="2"/>
@@ -1026,110 +1086,225 @@
       <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="J20" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K20" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L20" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M20" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B20">
+        <v>3.6668600000000003E-2</v>
+      </c>
+      <c r="C20">
+        <v>3.7277850000000001E-2</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.38719999999999999</v>
+      </c>
+      <c r="E20">
+        <v>40297</v>
+      </c>
+      <c r="F20">
+        <v>4229</v>
+      </c>
+      <c r="G20">
+        <v>36068</v>
+      </c>
+      <c r="H20">
+        <v>562</v>
+      </c>
+      <c r="I20">
+        <v>9638</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10494577760131027</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="1"/>
+        <v>0.8950542223986897</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" si="2"/>
+        <v>1.5581679050682045E-2</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="3"/>
+        <v>0.26721747809692803</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="J21" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K21" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L21" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M21" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B21">
+        <v>5.9065199999999998E-2</v>
+      </c>
+      <c r="C21">
+        <v>6.0315599999999997E-2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.1265</v>
+      </c>
+      <c r="E21">
+        <v>47221</v>
+      </c>
+      <c r="F21">
+        <v>1855</v>
+      </c>
+      <c r="G21">
+        <v>45366</v>
+      </c>
+      <c r="H21">
+        <v>612</v>
+      </c>
+      <c r="I21">
+        <v>12207</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="0"/>
+        <v>3.9283369687215436E-2</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="1"/>
+        <v>0.96071663031278454</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="2"/>
+        <v>1.3490279063615924E-2</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="3"/>
+        <v>0.26907816426398623</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="J22" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K22" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L22" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M22" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.18149999999999999</v>
+      </c>
+      <c r="E22">
+        <v>45206</v>
+      </c>
+      <c r="F22">
+        <v>2286</v>
+      </c>
+      <c r="G22">
+        <v>42930</v>
+      </c>
+      <c r="H22">
+        <v>662</v>
+      </c>
+      <c r="I22">
+        <v>11386</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="0"/>
+        <v>5.056850860505243E-2</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="1"/>
+        <v>0.94965270096889798</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="2"/>
+        <v>1.5420451898439319E-2</v>
+      </c>
+      <c r="M22" s="2">
+        <f t="shared" si="3"/>
+        <v>0.26522245515956205</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="J23" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K23" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L23" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M23" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B23">
+        <v>3.6501800000000001E-2</v>
+      </c>
+      <c r="C23">
+        <v>3.6501800000000001E-2</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="E23">
+        <v>43403</v>
+      </c>
+      <c r="F23">
+        <v>3883</v>
+      </c>
+      <c r="G23">
+        <v>39520</v>
+      </c>
+      <c r="H23">
+        <v>336</v>
+      </c>
+      <c r="I23">
+        <v>10688</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="0"/>
+        <v>8.946386194502684E-2</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="1"/>
+        <v>0.91053613805497313</v>
+      </c>
+      <c r="L23" s="2">
+        <f t="shared" si="2"/>
+        <v>8.5020242914979755E-3</v>
+      </c>
+      <c r="M23" s="2">
+        <f t="shared" si="3"/>
+        <v>0.27044534412955468</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="2"/>
-      <c r="J24" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K24" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L24" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M24" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.1719</v>
+      </c>
+      <c r="E24">
+        <v>49642</v>
+      </c>
+      <c r="F24">
+        <v>2211</v>
+      </c>
+      <c r="G24">
+        <v>47431</v>
+      </c>
+      <c r="H24">
+        <v>727</v>
+      </c>
+      <c r="I24">
+        <v>12441</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="0"/>
+        <v>4.4538898513355629E-2</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="1"/>
+        <v>0.95546110148664443</v>
+      </c>
+      <c r="L24" s="2">
+        <f t="shared" si="2"/>
+        <v>1.5327528409689865E-2</v>
+      </c>
+      <c r="M24" s="2">
+        <f t="shared" si="3"/>
+        <v>0.26229681010309713</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="3" customFormat="1">
@@ -1146,132 +1321,270 @@
       <c r="A26" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="J26" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K26" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L26" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M26" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B26">
+        <v>0.105839</v>
+      </c>
+      <c r="C26">
+        <v>0.107345</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.39950000000000002</v>
+      </c>
+      <c r="E26">
+        <v>36287</v>
+      </c>
+      <c r="F26">
+        <v>5884</v>
+      </c>
+      <c r="G26">
+        <v>30403</v>
+      </c>
+      <c r="H26">
+        <v>968</v>
+      </c>
+      <c r="I26">
+        <v>7620</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.16215173478105108</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="1"/>
+        <v>0.83784826521894895</v>
+      </c>
+      <c r="L26" s="2">
+        <f t="shared" si="2"/>
+        <v>3.1838963260204585E-2</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" si="3"/>
+        <v>0.25063316120119727</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="2"/>
-      <c r="J27" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K27" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L27" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M27" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B27">
+        <v>0.14574000000000001</v>
+      </c>
+      <c r="C27">
+        <v>0.14862</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.31490000000000001</v>
+      </c>
+      <c r="E27">
+        <v>36633</v>
+      </c>
+      <c r="F27">
+        <v>5891</v>
+      </c>
+      <c r="G27">
+        <v>30742</v>
+      </c>
+      <c r="H27">
+        <v>838</v>
+      </c>
+      <c r="I27">
+        <v>7546</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="0"/>
+        <v>0.16081129036660935</v>
+      </c>
+      <c r="K27" s="2">
+        <f t="shared" si="1"/>
+        <v>0.83918870963339065</v>
+      </c>
+      <c r="L27" s="2">
+        <f t="shared" si="2"/>
+        <v>2.725912432502765E-2</v>
+      </c>
+      <c r="M27" s="2">
+        <f t="shared" si="3"/>
+        <v>0.24546223407715828</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="J28" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K28" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L28" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M28" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B28">
+        <v>0.17979000000000001</v>
+      </c>
+      <c r="C28">
+        <v>0.18902099999999999</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="E28">
+        <v>44687</v>
+      </c>
+      <c r="F28">
+        <v>4676</v>
+      </c>
+      <c r="G28">
+        <v>40011</v>
+      </c>
+      <c r="H28">
+        <v>1080</v>
+      </c>
+      <c r="I28">
+        <v>9637</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10463893302302683</v>
+      </c>
+      <c r="K28" s="2">
+        <f t="shared" si="1"/>
+        <v>0.89536106697697315</v>
+      </c>
+      <c r="L28" s="2">
+        <f t="shared" si="2"/>
+        <v>2.699257704131364E-2</v>
+      </c>
+      <c r="M28" s="2">
+        <f t="shared" si="3"/>
+        <v>0.24085876383994401</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="2"/>
-      <c r="J29" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K29" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L29" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M29" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.26960000000000001</v>
+      </c>
+      <c r="E29">
+        <v>43323</v>
+      </c>
+      <c r="F29">
+        <v>4547</v>
+      </c>
+      <c r="G29">
+        <v>38776</v>
+      </c>
+      <c r="H29">
+        <v>1063</v>
+      </c>
+      <c r="I29">
+        <v>9387</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10495579715162846</v>
+      </c>
+      <c r="K29" s="2">
+        <f t="shared" si="1"/>
+        <v>0.8950442028483715</v>
+      </c>
+      <c r="L29" s="2">
+        <f t="shared" si="2"/>
+        <v>2.7413864245925314E-2</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="3"/>
+        <v>0.24208273158654839</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="J30" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K30" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L30" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M30" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B30">
+        <v>0.115005</v>
+      </c>
+      <c r="C30">
+        <v>0.108471</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.19350000000000001</v>
+      </c>
+      <c r="E30">
+        <v>46632</v>
+      </c>
+      <c r="F30">
+        <v>3824</v>
+      </c>
+      <c r="G30">
+        <v>42808</v>
+      </c>
+      <c r="H30">
+        <v>1085</v>
+      </c>
+      <c r="I30">
+        <v>10153</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="0"/>
+        <v>8.2003774232286844E-2</v>
+      </c>
+      <c r="K30" s="2">
+        <f t="shared" si="1"/>
+        <v>0.91799622576771311</v>
+      </c>
+      <c r="L30" s="2">
+        <f t="shared" si="2"/>
+        <v>2.5345729770136424E-2</v>
+      </c>
+      <c r="M30" s="2">
+        <f t="shared" si="3"/>
+        <v>0.237175294337507</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="2"/>
-      <c r="J31" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K31" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L31" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M31" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B31">
+        <v>0.19272</v>
+      </c>
+      <c r="C31">
+        <v>0.20850099999999999</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.3024</v>
+      </c>
+      <c r="E31">
+        <v>44480</v>
+      </c>
+      <c r="F31">
+        <v>4605</v>
+      </c>
+      <c r="G31">
+        <v>39875</v>
+      </c>
+      <c r="H31">
+        <v>1082</v>
+      </c>
+      <c r="I31">
+        <v>9596</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1035296762589928</v>
+      </c>
+      <c r="K31" s="2">
+        <f t="shared" si="1"/>
+        <v>0.89647032374100721</v>
+      </c>
+      <c r="L31" s="2">
+        <f t="shared" si="2"/>
+        <v>2.7134796238244514E-2</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" si="3"/>
+        <v>0.24065203761755485</v>
       </c>
     </row>
     <row r="32" spans="1:13" s="3" customFormat="1">
@@ -1288,158 +1601,322 @@
       <c r="A33" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="2"/>
-      <c r="J33" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K33" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L33" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M33" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B33">
+        <v>0.201206</v>
+      </c>
+      <c r="C33">
+        <v>0.20352300000000001</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.4027</v>
+      </c>
+      <c r="E33">
+        <v>26020</v>
+      </c>
+      <c r="F33">
+        <v>4844</v>
+      </c>
+      <c r="G33">
+        <v>21176</v>
+      </c>
+      <c r="H33">
+        <v>1212</v>
+      </c>
+      <c r="I33">
+        <v>5199</v>
+      </c>
+      <c r="J33" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18616448885472714</v>
+      </c>
+      <c r="K33" s="2">
+        <f t="shared" si="1"/>
+        <v>0.81383551114527286</v>
+      </c>
+      <c r="L33" s="2">
+        <f t="shared" si="2"/>
+        <v>5.723460521344919E-2</v>
+      </c>
+      <c r="M33" s="2">
+        <f t="shared" si="3"/>
+        <v>0.24551378919531544</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="2"/>
-      <c r="J34" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K34" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L34" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M34" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B34">
+        <v>0.316689</v>
+      </c>
+      <c r="C34">
+        <v>0.32125799999999999</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="E34">
+        <v>35287</v>
+      </c>
+      <c r="F34">
+        <v>3590</v>
+      </c>
+      <c r="G34">
+        <v>31697</v>
+      </c>
+      <c r="H34">
+        <v>1665</v>
+      </c>
+      <c r="I34">
+        <v>7097</v>
+      </c>
+      <c r="J34" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10173718366537252</v>
+      </c>
+      <c r="K34" s="2">
+        <f t="shared" si="1"/>
+        <v>0.89826281633462746</v>
+      </c>
+      <c r="L34" s="2">
+        <f t="shared" si="2"/>
+        <v>5.2528630469760543E-2</v>
+      </c>
+      <c r="M34" s="2">
+        <f t="shared" si="3"/>
+        <v>0.22390131558191628</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>12</v>
       </c>
-      <c r="D35" s="2"/>
-      <c r="J35" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K35" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L35" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M35" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B35">
+        <v>0.49959500000000001</v>
+      </c>
+      <c r="C35">
+        <v>0.55548699999999995</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.28370000000000001</v>
+      </c>
+      <c r="E35">
+        <v>31969</v>
+      </c>
+      <c r="F35">
+        <v>3450</v>
+      </c>
+      <c r="G35">
+        <v>28519</v>
+      </c>
+      <c r="H35">
+        <v>1366</v>
+      </c>
+      <c r="I35">
+        <v>6683</v>
+      </c>
+      <c r="J35" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10791704463699209</v>
+      </c>
+      <c r="K35" s="2">
+        <f t="shared" si="1"/>
+        <v>0.89208295536300797</v>
+      </c>
+      <c r="L35" s="2">
+        <f t="shared" si="2"/>
+        <v>4.7897892632981519E-2</v>
+      </c>
+      <c r="M35" s="2">
+        <f t="shared" si="3"/>
+        <v>0.23433500473368632</v>
       </c>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="2"/>
-      <c r="J36" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K36" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L36" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M36" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B36">
+        <v>0.14201</v>
+      </c>
+      <c r="C36">
+        <v>0.147228</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.25430000000000003</v>
+      </c>
+      <c r="E36">
+        <v>36389</v>
+      </c>
+      <c r="F36">
+        <v>3020</v>
+      </c>
+      <c r="G36">
+        <v>33369</v>
+      </c>
+      <c r="H36">
+        <v>1533</v>
+      </c>
+      <c r="I36">
+        <v>7323</v>
+      </c>
+      <c r="J36" s="2">
+        <f t="shared" si="0"/>
+        <v>8.2992113001181672E-2</v>
+      </c>
+      <c r="K36" s="2">
+        <f t="shared" si="1"/>
+        <v>0.9170078869988183</v>
+      </c>
+      <c r="L36" s="2">
+        <f t="shared" si="2"/>
+        <v>4.5940843297671494E-2</v>
+      </c>
+      <c r="M36" s="2">
+        <f t="shared" si="3"/>
+        <v>0.21945518295423896</v>
       </c>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="2"/>
-      <c r="J37" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K37" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L37" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M37" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B37">
+        <v>0.54125000000000001</v>
+      </c>
+      <c r="C37">
+        <v>0.59477599999999997</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.2276</v>
+      </c>
+      <c r="E37">
+        <v>38628</v>
+      </c>
+      <c r="F37">
+        <v>3365</v>
+      </c>
+      <c r="G37">
+        <v>35263</v>
+      </c>
+      <c r="H37">
+        <v>1660</v>
+      </c>
+      <c r="I37">
+        <v>7713</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="0"/>
+        <v>8.7112975044009527E-2</v>
+      </c>
+      <c r="K37" s="2">
+        <f t="shared" si="1"/>
+        <v>0.9128870249559905</v>
+      </c>
+      <c r="L37" s="2">
+        <f t="shared" si="2"/>
+        <v>4.7074837648526782E-2</v>
+      </c>
+      <c r="M37" s="2">
+        <f t="shared" si="3"/>
+        <v>0.21872784505005247</v>
       </c>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="2"/>
-      <c r="J38" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K38" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L38" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M38" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="B38">
+        <v>0.13164100000000001</v>
+      </c>
+      <c r="C38">
+        <v>0.14493</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.29289999999999999</v>
+      </c>
+      <c r="E38">
+        <v>29677</v>
+      </c>
+      <c r="F38">
+        <v>4865</v>
+      </c>
+      <c r="G38">
+        <v>24812</v>
+      </c>
+      <c r="H38">
+        <v>1371</v>
+      </c>
+      <c r="I38">
+        <v>5535</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="0"/>
+        <v>0.16393166425177746</v>
+      </c>
+      <c r="K38" s="2">
+        <f t="shared" si="1"/>
+        <v>0.83606833574822248</v>
+      </c>
+      <c r="L38" s="2">
+        <f t="shared" si="2"/>
+        <v>5.5255521521844271E-2</v>
+      </c>
+      <c r="M38" s="2">
+        <f t="shared" si="3"/>
+        <v>0.2230775431242947</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="2"/>
-      <c r="J39" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K39" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L39" s="2" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M39" s="2" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="D40" s="2"/>
+      <c r="B39">
+        <v>0.33652700000000002</v>
+      </c>
+      <c r="C39">
+        <v>0.33783200000000002</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.47549999999999998</v>
+      </c>
+      <c r="E39">
+        <v>23706</v>
+      </c>
+      <c r="F39">
+        <v>5706</v>
+      </c>
+      <c r="G39">
+        <v>18000</v>
+      </c>
+      <c r="H39">
+        <v>1090</v>
+      </c>
+      <c r="I39">
+        <v>4161</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="0"/>
+        <v>0.24069855732725892</v>
+      </c>
+      <c r="K39" s="2">
+        <f t="shared" si="1"/>
+        <v>0.75930144267274113</v>
+      </c>
+      <c r="L39" s="2">
+        <f t="shared" si="2"/>
+        <v>6.0555555555555557E-2</v>
+      </c>
+      <c r="M39" s="2">
+        <f t="shared" si="3"/>
+        <v>0.23116666666666666</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" s="3" customFormat="1">
+      <c r="A40" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="4"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -1447,57 +1924,162 @@
     </row>
     <row r="41" spans="1:13">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
+      <c r="J41" s="2" t="e">
+        <f t="shared" ref="J41:J47" si="4">F41/E41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K41" s="2" t="e">
+        <f t="shared" ref="K41:K47" si="5">G41/E41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L41" s="2" t="e">
+        <f t="shared" ref="L41:L47" si="6">H41/G41</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M41" s="2" t="e">
+        <f t="shared" ref="M41:M47" si="7">I41/G41</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="42" spans="1:13">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
       <c r="D42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
+      <c r="J42" s="2" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K42" s="2" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L42" s="2" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M42" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="43" spans="1:13">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
       <c r="D43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
+      <c r="J43" s="2" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K43" s="2" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L43" s="2" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M43" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="44" spans="1:13">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
       <c r="D44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
+      <c r="J44" s="2" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K44" s="2" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L44" s="2" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M44" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="45" spans="1:13">
+      <c r="A45" t="s">
+        <v>16</v>
+      </c>
       <c r="D45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
+      <c r="J45" s="2" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K45" s="2" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L45" s="2" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M45" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="46" spans="1:13">
+      <c r="A46" t="s">
+        <v>18</v>
+      </c>
       <c r="D46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
+      <c r="J46" s="2" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K46" s="2" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L46" s="2" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M46" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="47" spans="1:13">
+      <c r="A47" t="s">
+        <v>19</v>
+      </c>
       <c r="D47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
+      <c r="J47" s="2" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K47" s="2" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L47" s="2" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M47" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="48" spans="1:13">
+      <c r="A48" t="s">
+        <v>31</v>
+      </c>
       <c r="D48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
@@ -1547,7 +2129,6 @@
       <c r="M54" s="2"/>
     </row>
     <row r="55" spans="4:13">
-      <c r="D55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
@@ -1564,12 +2145,6 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
-    </row>
-    <row r="58" spans="4:13">
-      <c r="J58" s="2"/>
-      <c r="K58" s="2"/>
-      <c r="L58" s="2"/>
-      <c r="M58" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>